<commit_message>
update march and april books
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="773">
   <si>
     <t xml:space="preserve">Book</t>
   </si>
@@ -2300,7 +2300,7 @@
     <t xml:space="preserve">25-Feb</t>
   </si>
   <si>
-    <t xml:space="preserve">The Sweet Indeifference of the World</t>
+    <t xml:space="preserve">The Sweet Indifference of the World</t>
   </si>
   <si>
     <t xml:space="preserve">Peter Stamm</t>
@@ -2316,17 +2316,63 @@
   </si>
   <si>
     <t xml:space="preserve">5-Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucinella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore Segal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run to Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Yoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-Mar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Mysterious Affair at Styles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agatha Christie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-Apr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Hound of Baskervilles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arthur Conan Doyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19-Apr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Buried Giant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-May</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D;@"/>
     <numFmt numFmtId="166" formatCode="D\-MMM"/>
     <numFmt numFmtId="167" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="168" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -2431,10 +2477,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -2444,6 +2486,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2528,10 +2574,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K356"/>
+  <dimension ref="A1:K361"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A338" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A346" activeCellId="0" sqref="A346"/>
+      <selection pane="topLeft" activeCell="A360" activeCellId="0" sqref="A360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8632,7 +8678,7 @@
       <c r="A230" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B230" s="4" t="s">
+      <c r="B230" s="1" t="s">
         <v>507</v>
       </c>
       <c r="C230" s="1" t="s">
@@ -9256,7 +9302,7 @@
       <c r="A254" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="B254" s="4" t="s">
+      <c r="B254" s="1" t="s">
         <v>556</v>
       </c>
       <c r="C254" s="1" t="s">
@@ -9990,7 +10036,7 @@
       <c r="A282" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="B282" s="4" t="s">
+      <c r="B282" s="1" t="s">
         <v>607</v>
       </c>
       <c r="C282" s="1" t="s">
@@ -10760,8 +10806,8 @@
       <c r="I310" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J310" s="5"/>
-      <c r="K310" s="6"/>
+      <c r="J310" s="4"/>
+      <c r="K310" s="5"/>
     </row>
     <row r="311" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="s">
@@ -11004,7 +11050,7 @@
       <c r="A320" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="B320" s="4" t="s">
+      <c r="B320" s="1" t="s">
         <v>681</v>
       </c>
       <c r="C320" s="1" t="s">
@@ -11186,106 +11232,106 @@
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A327" s="7" t="s">
+      <c r="A327" s="6" t="s">
         <v>693</v>
       </c>
-      <c r="B327" s="7" t="s">
+      <c r="B327" s="6" t="s">
         <v>694</v>
       </c>
-      <c r="C327" s="7" t="s">
+      <c r="C327" s="6" t="s">
         <v>695</v>
       </c>
-      <c r="D327" s="7" t="s">
+      <c r="D327" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E327" s="3" t="n">
         <v>43666</v>
       </c>
-      <c r="F327" s="7" t="n">
+      <c r="F327" s="6" t="n">
         <v>2019</v>
       </c>
-      <c r="H327" s="7" t="n">
+      <c r="H327" s="6" t="n">
         <v>176</v>
       </c>
-      <c r="I327" s="7" t="s">
+      <c r="I327" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A328" s="7" t="s">
+      <c r="A328" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="B328" s="7" t="s">
+      <c r="B328" s="6" t="s">
         <v>697</v>
       </c>
-      <c r="C328" s="7" t="s">
+      <c r="C328" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D328" s="7" t="s">
+      <c r="D328" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E328" s="3" t="n">
         <v>43671</v>
       </c>
-      <c r="F328" s="7" t="n">
+      <c r="F328" s="6" t="n">
         <v>2019</v>
       </c>
-      <c r="H328" s="7" t="n">
+      <c r="H328" s="6" t="n">
         <v>198</v>
       </c>
-      <c r="I328" s="7" t="s">
+      <c r="I328" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A329" s="7" t="s">
+      <c r="A329" s="6" t="s">
         <v>698</v>
       </c>
-      <c r="B329" s="7" t="s">
+      <c r="B329" s="6" t="s">
         <v>699</v>
       </c>
-      <c r="C329" s="7" t="s">
+      <c r="C329" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D329" s="7" t="s">
+      <c r="D329" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E329" s="3" t="n">
         <v>43674</v>
       </c>
-      <c r="F329" s="7" t="n">
+      <c r="F329" s="6" t="n">
         <v>2019</v>
       </c>
-      <c r="H329" s="7" t="n">
+      <c r="H329" s="6" t="n">
         <v>228</v>
       </c>
-      <c r="I329" s="7" t="s">
+      <c r="I329" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A330" s="7" t="s">
+      <c r="A330" s="6" t="s">
         <v>700</v>
       </c>
-      <c r="B330" s="7" t="s">
+      <c r="B330" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="C330" s="7" t="s">
+      <c r="C330" s="6" t="s">
         <v>702</v>
       </c>
-      <c r="D330" s="7" t="s">
+      <c r="D330" s="6" t="s">
         <v>703</v>
       </c>
       <c r="E330" s="3" t="n">
         <v>43683</v>
       </c>
-      <c r="F330" s="7" t="n">
+      <c r="F330" s="6" t="n">
         <v>2019</v>
       </c>
-      <c r="H330" s="7" t="n">
+      <c r="H330" s="6" t="n">
         <v>252</v>
       </c>
-      <c r="I330" s="7" t="s">
+      <c r="I330" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -11969,6 +12015,136 @@
       </c>
       <c r="I356" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E357" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="F357" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H357" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="I357" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E358" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F358" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H358" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="I358" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E359" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="F359" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H359" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="I359" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E360" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="F360" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H360" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="I360" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E361" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="F361" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H361" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="I361" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
June and july books
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="781">
   <si>
     <t xml:space="preserve">Book</t>
   </si>
@@ -2361,6 +2361,30 @@
   </si>
   <si>
     <t xml:space="preserve">7-May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convenience Store Women</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sayaka Murata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Moonstone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilkie Collins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Name of the Rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umbero Eco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greenwood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Christie</t>
   </si>
 </sst>
 </file>
@@ -2574,10 +2598,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K361"/>
+  <dimension ref="A1:K365"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A338" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A360" activeCellId="0" sqref="A360"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A341" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E371" activeCellId="0" sqref="E371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12134,7 +12158,7 @@
       <c r="D361" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E361" s="1" t="s">
+      <c r="E361" s="7" t="s">
         <v>772</v>
       </c>
       <c r="F361" s="1" t="n">
@@ -12144,6 +12168,110 @@
         <v>345</v>
       </c>
       <c r="I361" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E362" s="7" t="n">
+        <v>43962</v>
+      </c>
+      <c r="F362" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H362" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="I362" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E363" s="7" t="n">
+        <v>43976</v>
+      </c>
+      <c r="F363" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H363" s="1" t="n">
+        <v>528</v>
+      </c>
+      <c r="I363" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E364" s="7" t="n">
+        <v>44013</v>
+      </c>
+      <c r="F364" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H364" s="1" t="n">
+        <v>611</v>
+      </c>
+      <c r="I364" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E365" s="7" t="n">
+        <v>44025</v>
+      </c>
+      <c r="F365" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H365" s="1" t="n">
+        <v>502</v>
+      </c>
+      <c r="I365" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>